<commit_message>
added json to Excel conversion
</commit_message>
<xml_diff>
--- a/FAIR_Metadata_Template.xlsx
+++ b/FAIR_Metadata_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aridhia/repos/fair-excel-to-json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B2A49-33A8-9446-BFF8-93F90636017C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0161759F-4E3E-EC41-8871-74DE07BB8E8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6680" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalogue" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -558,7 +558,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -607,7 +607,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -656,7 +656,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -705,7 +705,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -754,7 +754,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -803,7 +803,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -852,7 +852,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -901,7 +901,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -950,7 +950,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -999,7 +999,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1048,7 +1048,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1097,7 +1097,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1146,7 +1146,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1195,7 +1195,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1573,58 +1573,58 @@
     </row>
     <row r="7" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1634,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="B10" numberStoredAsText="1"/>
+    <ignoredError sqref="B8" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
New lookups structure in JSON
</commit_message>
<xml_diff>
--- a/FAIR_Metadata_Template.xlsx
+++ b/FAIR_Metadata_Template.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aridhia/repos/fair-excel-to-json/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertoverduin\Documents\Git\fair-excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDA2F20-C739-3B40-84F3-E31F27BAEF70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6040B5DE-3509-4225-A9CB-745FDDC1160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="648" yWindow="564" windowWidth="22224" windowHeight="10836" tabRatio="910" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="catalogue" sheetId="1" r:id="rId1"/>
-    <sheet name="dictionaries" sheetId="2" r:id="rId2"/>
-    <sheet name="fields" sheetId="3" r:id="rId3"/>
-    <sheet name="lookups" sheetId="4" r:id="rId4"/>
+    <sheet name="README" sheetId="7" r:id="rId1"/>
+    <sheet name="configuration" sheetId="6" r:id="rId2"/>
+    <sheet name="catalogue" sheetId="1" r:id="rId3"/>
+    <sheet name="dictionaries" sheetId="2" r:id="rId4"/>
+    <sheet name="fields" sheetId="3" r:id="rId5"/>
+    <sheet name="lookups" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -65,9 +67,6 @@
     <t>contactPoint</t>
   </si>
   <si>
-    <t>iris, flower, sepal, petal</t>
-  </si>
-  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -86,108 +85,21 @@
     <t>constraints</t>
   </si>
   <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>Internal identifier</t>
-  </si>
-  <si>
-    <t>sepal_length</t>
-  </si>
-  <si>
-    <t>Sepal Length</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>Sepal length in cm</t>
-  </si>
-  <si>
-    <t>sepal_width</t>
-  </si>
-  <si>
-    <t>Sepal Width</t>
-  </si>
-  <si>
-    <t>Sepal width in cm</t>
-  </si>
-  <si>
-    <t>petal_length</t>
-  </si>
-  <si>
-    <t>Petal Length</t>
-  </si>
-  <si>
-    <t>Petal length in cm</t>
-  </si>
-  <si>
-    <t>petal_width</t>
-  </si>
-  <si>
-    <t>Petal Width</t>
-  </si>
-  <si>
-    <t>Petal width in cm</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>SPECIES</t>
-  </si>
-  <si>
     <t>lookup</t>
   </si>
   <si>
-    <t>setosa</t>
-  </si>
-  <si>
-    <t>Iris setosa</t>
-  </si>
-  <si>
-    <t>versicolor</t>
-  </si>
-  <si>
-    <t>Iris versicolor</t>
-  </si>
-  <si>
-    <t>virginica</t>
-  </si>
-  <si>
-    <t>Iris virginica</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>key</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>a dessdsdsd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hi </t>
-  </si>
-  <si>
-    <t>Hi</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -197,83 +109,680 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Hi there</t>
-  </si>
-  <si>
     <t>SEX</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>Test Dataset</t>
-  </si>
-  <si>
-    <t>This is a test dataset. Originally published at UCI Machine Learning Repository: Iris Data Set, this small dataset from 1936 is often used for testing out machine learning algorithms and visualizations (for example, Scatter Plot). Each row of the table represents an iris flower, including its species and dimensions of its botanical parts, sepal and petal, in centimeters.</t>
-  </si>
-  <si>
-    <t>Gary McGilvary</t>
-  </si>
-  <si>
-    <t>gary.mcgilvary@aridhia.com</t>
-  </si>
-  <si>
     <t>Aridhia</t>
   </si>
   <si>
-    <t>aridhia.com</t>
-  </si>
-  <si>
-    <t>MIT</t>
-  </si>
-  <si>
-    <t>https://knowledgebase.aridhia.io/article/terms-and-conditions/</t>
-  </si>
-  <si>
-    <t>test description for test_dict_1</t>
-  </si>
-  <si>
-    <t>another test description for test_dict_2</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>test_dict_1</t>
-  </si>
-  <si>
-    <t>test_dict_2</t>
-  </si>
-  <si>
     <t>dictionary_id</t>
   </si>
   <si>
-    <t>Test Dictionary 1</t>
-  </si>
-  <si>
-    <t>Test Dictionary 2</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Bert Overduin</t>
+  </si>
+  <si>
+    <t>bert.overduin@aridhia.com</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/3.0/</t>
+  </si>
+  <si>
+    <t>http://aridhia.com</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Demographics data</t>
+  </si>
+  <si>
+    <t>Patient Id</t>
+  </si>
+  <si>
+    <t>APOE_GENOTYPE</t>
+  </si>
+  <si>
+    <t>apoe_genotype</t>
+  </si>
+  <si>
+    <t>APOE Genotype</t>
+  </si>
+  <si>
+    <t>apoe4_carrier</t>
+  </si>
+  <si>
+    <t>APOE4 Carrier</t>
+  </si>
+  <si>
+    <t>apoe4_alleles</t>
+  </si>
+  <si>
+    <t>APOE4 Alleles</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>APOE genotype</t>
+  </si>
+  <si>
+    <t>APOE4 carrier</t>
+  </si>
+  <si>
+    <t>APOE4 number of alleles</t>
+  </si>
+  <si>
+    <t>Patient identifier</t>
+  </si>
+  <si>
+    <t>Biological sex</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>apoe_date</t>
+  </si>
+  <si>
+    <t>APOE Date</t>
+  </si>
+  <si>
+    <t>APOE date</t>
+  </si>
+  <si>
+    <t>Test dataset</t>
+  </si>
+  <si>
+    <t>This test dataset consists of two tables, one containing demographics data and one containing APOE genotyping data.</t>
+  </si>
+  <si>
+    <t>APOE genotyping data</t>
+  </si>
+  <si>
+    <t>https://doi.org/</t>
+  </si>
+  <si>
+    <t>http://data.rights.aridhia.com</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>demographics,apoe</t>
+  </si>
+  <si>
+    <t>test_demographics</t>
+  </si>
+  <si>
+    <t>Test Demographics</t>
+  </si>
+  <si>
+    <t>test_apoe</t>
+  </si>
+  <si>
+    <t>Test APOE</t>
+  </si>
+  <si>
+    <t>e2/e2</t>
+  </si>
+  <si>
+    <t>e2/e3</t>
+  </si>
+  <si>
+    <t>e2/e4</t>
+  </si>
+  <si>
+    <t>e3/e3</t>
+  </si>
+  <si>
+    <t>e3/e4</t>
+  </si>
+  <si>
+    <t>e4/e4</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>visibility</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>PLEASE READ CAREFULLY BEFORE FILLING IN THIS TEMPLATE</t>
+  </si>
+  <si>
+    <t>lookups</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>dictionaries</t>
+  </si>
+  <si>
+    <t>catalogue</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <r>
+      <t>(4)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> should be separated by commas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(5)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> can only contain letters, numbers, and underscores, and cannot start with a number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(6)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>dictionary_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> should be taken from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> column of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>dictionaries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(7)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> can only contain letters, numbers, and underscores, and cannot start with a number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(10)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>lookup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> should be taken from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>constraints</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> column </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>can only contain letters, numbers, and underscores.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(2) Allowed values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>workflow_key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: these depend on which Data Access Requests are enabled on the hub in question, so this should be checked beforehand. If Data Access Requests aren't enabled, both the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>workflow_key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> key and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>workflow_key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> value should be removed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(1) Allowed values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>visibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: private, internal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(8) Allowed values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: boolean, date, datetime, decimal, integer, text, time.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(9) Variables of type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> boolean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> cannot have constraints.</t>
+    </r>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>APOE4_ALLELES</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>One APOE4 allele</t>
+  </si>
+  <si>
+    <t>Two APOE4 alleles</t>
+  </si>
+  <si>
+    <t>No APOE4 alleles</t>
+  </si>
+  <si>
+    <t>workflow_key</t>
+  </si>
+  <si>
+    <t>basic_access_request</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -348,6 +857,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -370,11 +892,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -400,12 +919,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -417,6 +930,36 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,7 +1056,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -562,7 +1105,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -611,7 +1154,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -660,7 +1203,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -709,7 +1252,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -758,7 +1301,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -807,7 +1350,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -856,7 +1399,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -905,7 +1448,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -954,7 +1497,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1003,7 +1546,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1052,7 +1595,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1101,7 +1644,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1150,7 +1693,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1199,7 +1742,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1505,495 +2048,739 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA9D668-8CDE-4707-A496-2FDFABA881ED}">
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1"/>
-    <col min="4" max="4" width="11.33203125" style="2"/>
-    <col min="5" max="5" width="12" style="3"/>
-    <col min="6" max="6" width="11.6640625" style="3"/>
-    <col min="7" max="7" width="14.33203125" style="3"/>
-    <col min="8" max="8" width="13.1640625" style="3"/>
-    <col min="9" max="9" width="12.6640625" style="3"/>
-    <col min="10" max="11" width="13.6640625" style="3"/>
-    <col min="12" max="12" width="14.6640625" style="3"/>
-    <col min="13" max="13" width="10.33203125" style="3"/>
-    <col min="14" max="14" width="17.5" style="3"/>
-    <col min="15" max="15" width="11.1640625" style="3"/>
-    <col min="16" max="1025" width="8.6640625" style="3"/>
-    <col min="1026" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" ht="128" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>68</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{8BB74521-D736-E240-9758-E4231344C275}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A3EED7-2FB2-1547-B2BC-D33363745521}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F322AE90-DC32-4BF9-8983-7AF157BFDE42}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
+      <c r="B2" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23744966-98F6-2D41-ABEE-DD2D7303C62A}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1"/>
+    <col min="4" max="4" width="12" style="2"/>
+    <col min="5" max="5" width="11.6640625" style="2"/>
+    <col min="6" max="6" width="14.33203125" style="2"/>
+    <col min="7" max="7" width="13.109375" style="2"/>
+    <col min="8" max="8" width="12.6640625" style="2"/>
+    <col min="9" max="10" width="13.6640625" style="2"/>
+    <col min="11" max="11" width="14.6640625" style="2"/>
+    <col min="12" max="12" width="10.33203125" style="2"/>
+    <col min="13" max="13" width="17.44140625" style="2"/>
+    <col min="14" max="14" width="11.109375" style="2"/>
+    <col min="15" max="1024" width="8.6640625" style="2"/>
+    <col min="1025" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{8BB74521-D736-E240-9758-E4231344C275}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{C0E02ED8-F4D1-4AB8-A807-6100759D11F4}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{28FE65B1-7AD6-44E9-8F39-800E6984C31B}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{FDE95023-F4F9-4FC9-876C-2877CA79DC94}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{B8F3EE1A-C57B-47DD-B2C0-8931C528AC68}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="B8" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700AEE39-DD6B-D64B-9A4F-73DDF6E54D4B}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A3EED7-2FB2-1547-B2BC-D33363745521}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="11.5546875" style="18"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>14</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="15" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>60</v>
-      </c>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23744966-98F6-2D41-ABEE-DD2D7303C62A}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700AEE39-DD6B-D64B-9A4F-73DDF6E54D4B}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
+  </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="B11:B13" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced catalogue id by dataset code
</commit_message>
<xml_diff>
--- a/FAIR_Metadata_Template.xlsx
+++ b/FAIR_Metadata_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertoverduin\Documents\Git\fair-excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DCDFF3-E8DC-425C-8914-DCAC04344283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0316A268-0100-44A4-8DB5-0D66DC03B31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1176" windowWidth="20364" windowHeight="10740" tabRatio="910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="144" yWindow="204" windowWidth="20952" windowHeight="11016" tabRatio="910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Aridhia</t>
   </si>
   <si>
-    <t>dictionary_id</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Bert Overduin</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>APOE date</t>
   </si>
   <si>
-    <t>Test dataset</t>
-  </si>
-  <si>
     <t>This test dataset consists of two tables, one containing demographics data and one containing APOE genotyping data.</t>
   </si>
   <si>
@@ -229,13 +220,7 @@
     <t>test_demographics</t>
   </si>
   <si>
-    <t>Test Demographics</t>
-  </si>
-  <si>
     <t>test_apoe</t>
-  </si>
-  <si>
-    <t>Test APOE</t>
   </si>
   <si>
     <t>e2/e2</t>
@@ -400,9 +385,6 @@
     <t>basic_access_request</t>
   </si>
   <si>
-    <t>This field is MANDATORY!</t>
-  </si>
-  <si>
     <r>
       <t>(11)</t>
     </r>
@@ -580,7 +562,7 @@
   </si>
   <si>
     <r>
-      <t>(7)</t>
+      <t>(5)</t>
     </r>
     <r>
       <rPr>
@@ -600,7 +582,7 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>dictionary_id</t>
+      <t>keywords</t>
     </r>
     <r>
       <rPr>
@@ -610,7 +592,12 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> should be taken from the </t>
+      <t xml:space="preserve"> should be separated by commas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(3) </t>
     </r>
     <r>
       <rPr>
@@ -620,16 +607,16 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> column of the </t>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -639,31 +626,16 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>dictionaries</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sheet.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(6)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
     </r>
     <r>
       <rPr>
@@ -673,31 +645,30 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> can only contain letters, numbers, and underscores, and cannot start with a number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(5)</t>
+      <t>publisher_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> are mandatory fields.</t>
+    </r>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3)</t>
     </r>
     <r>
       <rPr>
@@ -717,28 +688,46 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>keywords</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> should be separated by commas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(4)</t>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>can only contain letters, numbers, and underscores.</t>
+    </r>
+  </si>
+  <si>
+    <t>test_dataset</t>
+  </si>
+  <si>
+    <t>Test Demographics</t>
+  </si>
+  <si>
+    <t>Test APOE</t>
+  </si>
+  <si>
+    <t>Test Dataset</t>
+  </si>
+  <si>
+    <t>dictionary_code</t>
+  </si>
+  <si>
+    <r>
+      <t>(6)</t>
     </r>
     <r>
       <rPr>
@@ -758,7 +747,31 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>id</t>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> can only contain letters, numbers, and underscores, and cannot start with a number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(7)</t>
     </r>
     <r>
       <rPr>
@@ -769,20 +782,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>can only contain letters, numbers, and underscores.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(3) </t>
     </r>
     <r>
       <rPr>
@@ -792,16 +791,17 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>title</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
+      <t>dictionary_code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> should be taken from the </t>
     </r>
     <r>
       <rPr>
@@ -811,16 +811,16 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>description</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, and </t>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> column of the </t>
     </r>
     <r>
       <rPr>
@@ -830,16 +830,16 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>publisher_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> are mandatory fields.</t>
+      <t>dictionaries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet.</t>
     </r>
   </si>
 </sst>
@@ -847,7 +847,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -864,13 +864,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF767171"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -955,74 +948,71 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1121,9 +1111,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1170,9 +1160,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1219,9 +1209,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1268,9 +1258,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1317,9 +1307,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1366,9 +1356,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1415,9 +1405,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1464,9 +1454,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1513,9 +1503,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1562,9 +1552,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1611,9 +1601,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1660,9 +1650,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1709,9 +1699,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1758,9 +1748,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1807,9 +1797,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2116,105 +2106,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA9D668-8CDE-4707-A496-2FDFABA881ED}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="53.109375" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>84</v>
+      <c r="A4" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>83</v>
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A7" s="24"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
-        <v>99</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>98</v>
+      <c r="A17" s="25" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>97</v>
+      <c r="A18" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>96</v>
+      <c r="A19" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
-        <v>78</v>
+      <c r="A21" s="24" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
-        <v>95</v>
+      <c r="A22" s="25" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2228,41 +2221,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F322AE90-DC32-4BF9-8983-7AF157BFDE42}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="17.77734375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>76</v>
+      <c r="A2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>93</v>
+      <c r="A3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2276,151 +2277,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AMI12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2"/>
-    <col min="5" max="5" width="11.6640625" style="2"/>
-    <col min="6" max="6" width="14.33203125" style="2"/>
-    <col min="7" max="7" width="13.109375" style="2"/>
-    <col min="8" max="8" width="12.6640625" style="2"/>
-    <col min="9" max="10" width="13.6640625" style="2"/>
-    <col min="11" max="11" width="14.6640625" style="2"/>
-    <col min="12" max="12" width="10.33203125" style="2"/>
-    <col min="13" max="13" width="17.44140625" style="2"/>
-    <col min="14" max="14" width="11.109375" style="2"/>
-    <col min="15" max="1024" width="8.6640625" style="2"/>
-    <col min="1025" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="23.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1"/>
+    <col min="5" max="5" width="14.33203125" style="1"/>
+    <col min="6" max="6" width="13.109375" style="1"/>
+    <col min="7" max="7" width="12.6640625" style="1"/>
+    <col min="8" max="9" width="13.6640625" style="1"/>
+    <col min="10" max="10" width="14.6640625" style="1"/>
+    <col min="11" max="11" width="10.33203125" style="1"/>
+    <col min="12" max="12" width="17.44140625" style="1"/>
+    <col min="13" max="13" width="11.109375" style="1"/>
+    <col min="14" max="1023" width="8.6640625" style="1"/>
+    <col min="1024" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="6" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{8BB74521-D736-E240-9758-E4231344C275}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{C0E02ED8-F4D1-4AB8-A807-6100759D11F4}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{28FE65B1-7AD6-44E9-8F39-800E6984C31B}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{FDE95023-F4F9-4FC9-876C-2877CA79DC94}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{B8F3EE1A-C57B-47DD-B2C0-8931C528AC68}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{8BB74521-D736-E240-9758-E4231344C275}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{C0E02ED8-F4D1-4AB8-A807-6100759D11F4}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{28FE65B1-7AD6-44E9-8F39-800E6984C31B}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{FDE95023-F4F9-4FC9-876C-2877CA79DC94}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{B8F3EE1A-C57B-47DD-B2C0-8931C528AC68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -2428,7 +2411,7 @@
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Protective Marking: Internal</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B8" numberStoredAsText="1"/>
+    <ignoredError sqref="B7" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId7"/>
 </worksheet>
@@ -2438,53 +2421,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A3EED7-2FB2-1547-B2BC-D33363745521}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="18"/>
+    <col min="1" max="1" width="18.77734375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="17" customWidth="1"/>
+    <col min="4" max="16384" width="11.5546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
+      <c r="A2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>59</v>
+      <c r="A3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2499,9 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23744966-98F6-2D41-ABEE-DD2D7303C62A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2509,179 +2488,179 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="15" customWidth="1"/>
     <col min="6" max="6" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="C7" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="22" t="s">
+      <c r="E9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2704,152 +2683,152 @@
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>